<commit_message>
mod guangdong gather to sorghum and barley
</commit_message>
<xml_diff>
--- a/database/CFTCopi.xlsx
+++ b/database/CFTCopi.xlsx
@@ -89,45 +89,51 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -142,21 +148,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -172,14 +172,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -202,31 +203,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -241,13 +241,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +385,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,151 +421,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,26 +432,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -466,39 +446,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -532,6 +479,59 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -540,10 +540,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -552,137 +552,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -703,6 +703,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -1058,7 +1061,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D684" sqref="D684"/>
+      <selection pane="bottomRight" activeCell="E681" sqref="E681"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -29121,20 +29124,46 @@
       </c>
       <c r="N678" s="3"/>
     </row>
-    <row r="679" spans="1:14">
-      <c r="A679" s="3"/>
-      <c r="B679" s="3"/>
-      <c r="C679" s="3"/>
-      <c r="D679" s="3"/>
-      <c r="E679" s="3"/>
-      <c r="F679" s="3"/>
-      <c r="G679" s="3"/>
-      <c r="H679" s="6"/>
-      <c r="I679" s="3"/>
-      <c r="J679" s="3"/>
-      <c r="K679" s="3"/>
-      <c r="L679" s="3"/>
-      <c r="M679" s="3"/>
+    <row r="679" ht="15" spans="1:14">
+      <c r="A679" s="5">
+        <v>43613</v>
+      </c>
+      <c r="B679" s="10">
+        <v>1818382</v>
+      </c>
+      <c r="C679" s="10">
+        <v>233812</v>
+      </c>
+      <c r="D679" s="10">
+        <v>256106</v>
+      </c>
+      <c r="E679" s="10">
+        <v>444957</v>
+      </c>
+      <c r="F679" s="10">
+        <v>85887</v>
+      </c>
+      <c r="G679" s="10">
+        <v>109093</v>
+      </c>
+      <c r="H679" s="9">
+        <v>328319</v>
+      </c>
+      <c r="I679" s="10">
+        <v>50850</v>
+      </c>
+      <c r="J679" s="10">
+        <v>91224</v>
+      </c>
+      <c r="K679" s="10">
+        <v>778621</v>
+      </c>
+      <c r="L679" s="10">
+        <v>64252</v>
+      </c>
+      <c r="M679" s="10">
+        <v>192389</v>
+      </c>
       <c r="N679" s="3"/>
     </row>
     <row r="680" spans="1:14">

</xml_diff>